<commit_message>
bill model in separate file
</commit_message>
<xml_diff>
--- a/GV compta plomberie.xlsx
+++ b/GV compta plomberie.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="je suis sous l'eau" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Robert &amp; fils" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -345,7 +346,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -356,37 +357,37 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>work_type</t>
+          <t>Type de traveaux</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>company_name</t>
+          <t>Nom de l'entreprise</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>comment</t>
+          <t>Commentaire</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>start_date</t>
+          <t>Date de debut des traveaux</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>end_date</t>
+          <t>Date de fin des traveaux</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>price</t>
+          <t>Prix</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>work_status</t>
+          <t>Etat du payment</t>
         </is>
       </c>
     </row>
@@ -403,27 +404,27 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Tuyaux au sous sol de C4. </t>
+          <t>Remplacer le robinet au sous sol du B3. Travail effectué, facture payé.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>15.09.2019</t>
+          <t>04.11.2019</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>17.09.2019</t>
+          <t>04.11.2019</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>350.69</t>
+          <t>300</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Started</t>
+          <t>Payé</t>
         </is>
       </c>
     </row>
@@ -440,27 +441,157 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Robinet d'eau Bat. B2.</t>
+          <t>test</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>17.09.2019</t>
+          <t>04.11.2019</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>17.09.2019</t>
+          <t>04.11.2019</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>150.36</t>
+          <t>365</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Finished</t>
+          <t>Payé</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>plomberie</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>je suis sous l'eau</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>test1</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>04.11.2019</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>04.11.2019</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Payé</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Type de traveaux</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Nom de l'entreprise</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Commentaire</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Date de debut des traveaux</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Date de fin des traveaux</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Prix</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Etat du payment</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>plomberie</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Robert &amp; fils</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Changement du radiateur dans la loge de gardien. Fait, payé.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>04.11.2019</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>10.11.2019</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Payé</t>
         </is>
       </c>
     </row>

</xml_diff>